<commit_message>
Fix inconsistent capitalization in nodes
This introduced an issue with the SVG behind the layout which is fixed in this commit - should be much more stable now
</commit_message>
<xml_diff>
--- a/scripts/connections.xlsx
+++ b/scripts/connections.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="186">
   <si>
     <t xml:space="preserve">UCC</t>
   </si>
@@ -52,28 +52,28 @@
     <t xml:space="preserve">UCC1</t>
   </si>
   <si>
-    <t xml:space="preserve">Restoring and maintaining the water cycle</t>
+    <t xml:space="preserve">Restoring and Maintaining the Water Cycle</t>
   </si>
   <si>
     <t xml:space="preserve">D1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Alternative water source RW</t>
+    <t xml:space="preserve">Alternative Water Source RW</t>
   </si>
   <si>
     <t xml:space="preserve">S1.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Collection/Conveyance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filter strips</t>
+    <t xml:space="preserve">Collection / Conveyance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter Strips</t>
   </si>
   <si>
     <t xml:space="preserve">A filter strip is a sloped medium that attenuates stormwater runoff by converting it into sheet flow, typically located parallel to an impervious surface such as a parking lot, driveway, or roadway. Adapted from UACDC (2010).</t>
   </si>
   <si>
-    <t xml:space="preserve">Filter drain</t>
+    <t xml:space="preserve">Filter Drain</t>
   </si>
   <si>
     <t xml:space="preserve">Filter drains are shallow trenches filled with stone/gravel that create temporary subsurface storage for attenuation, conveyance and filtration of surface water runoff. The stone may be contained in a simple trench lined with a geotextile, geomembrane or other impermeable liner, or with a more structural facility such as a concrete trough. Adapted from Ballard et al. (2015).</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">A Bioswale is a vegetated, linear and low sloped pit, often established in urban areas. It is designed to store and convey surface water runoff and also remove pollutants and sediments. This NBS is often used to drain roads, paths or car parks while enhancing access corridors or other open space (adapted from URBANGREENUP (2018), NATURE4CITIES (2020), UNALAB (2019)).</t>
   </si>
   <si>
-    <t xml:space="preserve">Dry swale</t>
+    <t xml:space="preserve">Dry Swale</t>
   </si>
   <si>
     <t xml:space="preserve">A dry swale, or grassed swale, is an open grassed conveyance channel that filters, attenuates, and detains stormwater runoff as it moves downstream. Adapted from UACDC (2010).</t>
@@ -100,13 +100,13 @@
     <t xml:space="preserve">Treatment (RW)</t>
   </si>
   <si>
-    <t xml:space="preserve">Bioretention cell (Rain garden)</t>
+    <t xml:space="preserve">Bioretention Cell (Rain Garden)</t>
   </si>
   <si>
     <t xml:space="preserve">A bioretention cell is a shallow depressed vegetated area that primarily serves as area for water control (storage and infiltration) on a small-scale especially in urban areas. It is designed to collect, store, filter and treat water runoff. Storm water runoff is drained, stored for a certain period, and then it infiltrates either into the ground soil or flows into the sewage system. To optimise its functions, it must include a porous soil mixture, native vegetation and some hyper accumulator plants, capable of phyto-remediation. Adapted from URBANGREENUP (2018), UNALAB (2019).</t>
   </si>
   <si>
-    <t xml:space="preserve">Treatment wetland</t>
+    <t xml:space="preserve">Treatment Wetland</t>
   </si>
   <si>
     <t xml:space="preserve">Treatment wetlands (TWs) include a range of engineered systems designed and constructed to replicate natural processes occurring in natural wetlands involving vegetation, soils, and the associated microbial assemblages to assist in treating wastewater streams (e.g. domestic wastewater, greywater, industrial wastewater) and stormwater. TWs can be divided in two main hydrological categories: Free water surface wetlands, a shallow sealed basin or sequence of basins (open water areas) containing floating plants, submerged plants or emergent plants (similar in appearance to natural marshes); Subsurface flow wetlands, which include Horizontal flow (HF) wetlands and Vertical flow (VF) wetlands. In this case, the water flows beneath the surface level, either horizontally or vertically, through the filter bed. Adapted from URBANGREENUP (2018), NATURE4CITIES (2020), UNALAB (2019), Somarakis et al. (2019) and Dotro et al. (2017). </t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">Storage (RW)</t>
   </si>
   <si>
-    <t xml:space="preserve">(Wet) Retention pond</t>
+    <t xml:space="preserve">(Wet) Retention Pond</t>
   </si>
   <si>
     <r>
@@ -172,7 +172,7 @@
     <t xml:space="preserve">S2</t>
   </si>
   <si>
-    <t xml:space="preserve">Detention vaults and tanks</t>
+    <t xml:space="preserve">Detention Vaults and Tanks</t>
   </si>
   <si>
     <r>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">D1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Sustainable rainwater management</t>
+    <t xml:space="preserve">Sustainable Rainwater Management</t>
   </si>
   <si>
     <t xml:space="preserve">S1.2.1</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">Detention</t>
   </si>
   <si>
-    <t xml:space="preserve">Extensive green roof</t>
+    <t xml:space="preserve">Extensive Green Roof</t>
   </si>
   <si>
     <r>
@@ -232,7 +232,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Intensive green roof</t>
+    <t xml:space="preserve">Intensive Green Roof</t>
   </si>
   <si>
     <r>
@@ -256,7 +256,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">(Dry) Detention pond</t>
+    <t xml:space="preserve">(Dry) Detention Pond</t>
   </si>
   <si>
     <r>
@@ -280,7 +280,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">River restoration </t>
+    <t xml:space="preserve">River Restoration </t>
   </si>
   <si>
     <r>
@@ -334,7 +334,7 @@
     <t xml:space="preserve">Infiltration</t>
   </si>
   <si>
-    <t xml:space="preserve">Infiltration basin</t>
+    <t xml:space="preserve">Infiltration Basin</t>
   </si>
   <si>
     <r>
@@ -358,7 +358,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Infiltration trench</t>
+    <t xml:space="preserve">Infiltration Trench</t>
   </si>
   <si>
     <r>
@@ -382,7 +382,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Tree pits </t>
+    <t xml:space="preserve">Tree Pits</t>
   </si>
   <si>
     <r>
@@ -406,7 +406,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Vegetated grid pavement</t>
+    <t xml:space="preserve">Vegetated Grid Pavement</t>
   </si>
   <si>
     <r>
@@ -457,7 +457,7 @@
     <t xml:space="preserve">Evapotranspiration</t>
   </si>
   <si>
-    <t xml:space="preserve">Ground-based green facade </t>
+    <t xml:space="preserve">Ground-Based Green Facade </t>
   </si>
   <si>
     <r>
@@ -481,7 +481,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Wall-based green facade </t>
+    <t xml:space="preserve">Wall-Based Green Facade </t>
   </si>
   <si>
     <r>
@@ -505,7 +505,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Pot-based green facade </t>
+    <t xml:space="preserve">Pot-Based Green Facade </t>
   </si>
   <si>
     <r>
@@ -529,7 +529,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Semi-intensive green roof</t>
+    <t xml:space="preserve">Semi-Intensive Green Roof</t>
   </si>
   <si>
     <r>
@@ -553,7 +553,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Vegetated pergola</t>
+    <t xml:space="preserve">Vegetated Pergola</t>
   </si>
   <si>
     <r>
@@ -580,25 +580,25 @@
     <t xml:space="preserve">UCC2</t>
   </si>
   <si>
-    <t xml:space="preserve">Water and waste treatment and recovery</t>
+    <t xml:space="preserve">Water and Waste Treatment and Recovery</t>
   </si>
   <si>
     <t xml:space="preserve">D2.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Alternative water source WW</t>
+    <t xml:space="preserve">Alternative Water Source WW</t>
   </si>
   <si>
     <t xml:space="preserve">S2.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Collection/Separation</t>
+    <t xml:space="preserve">Collection / Separation</t>
   </si>
   <si>
     <t xml:space="preserve">S7</t>
   </si>
   <si>
-    <t xml:space="preserve">Physical unit operations for solid/liquid separation</t>
+    <t xml:space="preserve">Physical Unit Operations for Solid / Liquid Separation</t>
   </si>
   <si>
     <r>
@@ -628,28 +628,7 @@
     <t xml:space="preserve">Treatment (WW)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Treatment wetland</t>
-    </r>
-    <r>
-      <rPr>
-        <strike val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Anaerobic treatment (for nutrient, VFA &amp; methane recovery)</t>
+    <t xml:space="preserve">Anaerobic Treatment (for Nutrient, VFA &amp; Methane Recovery)</t>
   </si>
   <si>
     <r>
@@ -674,7 +653,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Waste stabilisation pond</t>
+    <t xml:space="preserve">Waste Stabilisation Pond</t>
   </si>
   <si>
     <t xml:space="preserve">﻿Waste stabilization ponds (WSPs) are earthen ponds designed and constructed in series, where sequential microbial metabolisms (anaerobic + facultative + aerobic) are established. WSPs utilize both physical and biological processes to remove organic materials, pollutants, and pathogens in raw wastewater. The size of the infrastructure can be comparable to a treatment wetland unit in some cases, and it can be applied also for cities. Adapted</t>
@@ -692,13 +671,13 @@
     <t xml:space="preserve">UCC3</t>
   </si>
   <si>
-    <t xml:space="preserve">Nutrient recovery and reuse</t>
+    <t xml:space="preserve">Nutrient Recovery and Reuse</t>
   </si>
   <si>
     <t xml:space="preserve">D3.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Alternative nutrient source from Wastewater</t>
+    <t xml:space="preserve">Alternative Nutrient Source From Wastewater</t>
   </si>
   <si>
     <t xml:space="preserve">S3.1.1</t>
@@ -707,7 +686,7 @@
     <t xml:space="preserve">Collection (WW)</t>
   </si>
   <si>
-    <t xml:space="preserve">Physical unit operations for streams separation (dedicated sewage systems)</t>
+    <t xml:space="preserve">Physical Unit Operations for Streams Separation (Dedicated Sewage Systems)</t>
   </si>
   <si>
     <r>
@@ -731,9 +710,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Treatment wetland </t>
-  </si>
-  <si>
     <t xml:space="preserve">Phytoremediation</t>
   </si>
   <si>
@@ -767,7 +743,7 @@
     <t xml:space="preserve">S3</t>
   </si>
   <si>
-    <t xml:space="preserve">Phosphate precipitation (for P recovery)</t>
+    <t xml:space="preserve">Phosphate Precipitation (for P Recovery)</t>
   </si>
   <si>
     <r>
@@ -794,7 +770,7 @@
     <t xml:space="preserve">S4</t>
   </si>
   <si>
-    <t xml:space="preserve">Ammonia stripping (for N recovery)</t>
+    <t xml:space="preserve">Ammonia Stripping (for N Recovery)</t>
   </si>
   <si>
     <r>
@@ -879,7 +855,7 @@
     <t xml:space="preserve">D3.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Alternative nutrient source from Food Waste</t>
+    <t xml:space="preserve">Alternative Nutrient Source From Food Waste</t>
   </si>
   <si>
     <t xml:space="preserve">S3.2.1</t>
@@ -918,7 +894,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Productive garden</t>
+    <t xml:space="preserve">Productive Garden</t>
   </si>
   <si>
     <r>
@@ -942,7 +918,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Urban farms and orchards</t>
+    <t xml:space="preserve">Urban Farms and Orchards</t>
   </si>
   <si>
     <r>
@@ -966,7 +942,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Urban forest</t>
+    <t xml:space="preserve">Urban Forest</t>
   </si>
   <si>
     <r>
@@ -990,7 +966,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Soil improvement and conservation</t>
+    <t xml:space="preserve">Soil Improvement and Conservation</t>
   </si>
   <si>
     <t xml:space="preserve">Coming soon!</t>
@@ -1002,7 +978,7 @@
     <t xml:space="preserve">UCC5</t>
   </si>
   <si>
-    <t xml:space="preserve">Food and biomass production</t>
+    <t xml:space="preserve">Food and Biomass Production</t>
   </si>
   <si>
     <t xml:space="preserve">D5.1</t>
@@ -1011,7 +987,7 @@
     <t xml:space="preserve">S5.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Production of edible BM</t>
+    <t xml:space="preserve">Production of Edible BM</t>
   </si>
   <si>
     <t xml:space="preserve">Aquaculture</t>
@@ -1038,7 +1014,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Hydroponic and soilless technologies</t>
+    <t xml:space="preserve">Hydroponic and Soilless Technologies</t>
   </si>
   <si>
     <r>
@@ -1087,7 +1063,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Aquaponic farming</t>
+    <t xml:space="preserve">Aquaponic Farming</t>
   </si>
   <si>
     <r>
@@ -1114,10 +1090,13 @@
     <t xml:space="preserve">S5.1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Production of non-edible BM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green corridors</t>
+    <t xml:space="preserve">Production of Inedible BM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urban forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green Corridors</t>
   </si>
   <si>
     <r>
@@ -1141,7 +1120,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Large urban park</t>
+    <t xml:space="preserve">Large Urban Park</t>
   </si>
   <si>
     <r>
@@ -1165,7 +1144,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Urban meadows</t>
+    <t xml:space="preserve">Urban Meadows</t>
   </si>
   <si>
     <r>
@@ -1210,16 +1189,16 @@
     <t xml:space="preserve">D5.3</t>
   </si>
   <si>
-    <t xml:space="preserve">Biomass waste harvesting (from all NBS)</t>
+    <t xml:space="preserve">Biomass Waste Harvesting (from all NBS)</t>
   </si>
   <si>
     <t xml:space="preserve">S5.3.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Biomass recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street trees</t>
+    <t xml:space="preserve">Biomass Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street Trees</t>
   </si>
   <si>
     <r>
@@ -1246,49 +1225,46 @@
     <t xml:space="preserve">UCC6</t>
   </si>
   <si>
-    <t xml:space="preserve">Energy efficiency and recovery</t>
+    <t xml:space="preserve">Energy Efficiency and Recovery</t>
   </si>
   <si>
     <t xml:space="preserve">D6.1</t>
   </si>
   <si>
-    <t xml:space="preserve">UHI mitigation/reduction</t>
+    <t xml:space="preserve">UHI Mitigation / Reduction</t>
   </si>
   <si>
     <t xml:space="preserve">S6.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Microclimate regulation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soil/ground-based green facade </t>
+    <t xml:space="preserve">Microclimate Regulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil / Ground-Based Green Facade </t>
   </si>
   <si>
     <t xml:space="preserve">D6.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Increase energy sufficiency</t>
+    <t xml:space="preserve">Increase Energy Sufficiency</t>
   </si>
   <si>
     <t xml:space="preserve">S6.2.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Increase building insulation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extensive green roof</t>
+    <t xml:space="preserve">Increase Building Insulation</t>
   </si>
   <si>
     <t xml:space="preserve">S6.2.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Energy recovery from biomass</t>
+    <t xml:space="preserve">Energy Recovery From Biomass</t>
   </si>
   <si>
     <t xml:space="preserve">S6.2.3</t>
   </si>
   <si>
-    <t xml:space="preserve">Energy recovery from Wastewater</t>
+    <t xml:space="preserve">Energy Recovery From Wastewater</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1274,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1380,13 +1356,6 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <strike val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1533,7 +1502,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1678,34 +1647,30 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1714,26 +1679,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1750,11 +1715,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1794,7 +1759,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1898,8 +1863,8 @@
   </sheetPr>
   <dimension ref="A1:I172"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H183" activeCellId="0" sqref="H183"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B113" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C128" activeCellId="0" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2625,7 +2590,7 @@
         <v>21</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="I59" s="8" t="s">
         <v>29</v>
@@ -2637,10 +2602,10 @@
         <v>26</v>
       </c>
       <c r="H60" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I60" s="29" t="s">
         <v>89</v>
-      </c>
-      <c r="I60" s="29" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2673,10 +2638,10 @@
         <v>22</v>
       </c>
       <c r="H63" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I63" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="I63" s="9" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2703,10 +2668,10 @@
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F67" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="G67" s="30" t="s">
         <v>37</v>
@@ -2715,7 +2680,7 @@
         <v>38</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2783,31 +2748,31 @@
     </row>
     <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="C75" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="D75" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="E75" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="F75" s="32" t="s">
         <v>100</v>
-      </c>
-      <c r="F75" s="32" t="s">
-        <v>101</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H75" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="I75" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="I75" s="13" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2815,11 +2780,11 @@
       <c r="G76" s="34" t="n">
         <v>26</v>
       </c>
-      <c r="H76" s="33" t="s">
+      <c r="H76" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I76" s="29" t="s">
         <v>89</v>
-      </c>
-      <c r="I76" s="29" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2828,7 +2793,7 @@
         <v>21</v>
       </c>
       <c r="H77" s="33" t="s">
-        <v>104</v>
+        <v>28</v>
       </c>
       <c r="I77" s="8" t="s">
         <v>29</v>
@@ -2840,10 +2805,10 @@
         <v>25</v>
       </c>
       <c r="H78" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I78" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,31 +2820,31 @@
     </row>
     <row r="80" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="F80" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="G80" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F80" s="32" t="s">
+      <c r="H80" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="G80" s="4" t="s">
+      <c r="I80" s="13" t="s">
         <v>109</v>
-      </c>
-      <c r="H80" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="I80" s="13" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F81" s="32"/>
       <c r="G81" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="H81" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="I81" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="H81" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="I81" s="13" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2887,11 +2852,11 @@
       <c r="G82" s="34" t="n">
         <v>26</v>
       </c>
-      <c r="H82" s="33" t="s">
+      <c r="H82" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I82" s="29" t="s">
         <v>89</v>
-      </c>
-      <c r="I82" s="29" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2900,22 +2865,22 @@
         <v>48</v>
       </c>
       <c r="H83" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I83" s="29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F84" s="32"/>
       <c r="G84" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="H84" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="I84" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="H84" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="I84" s="13" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,10 +2889,10 @@
         <v>25</v>
       </c>
       <c r="H85" s="37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2944,10 +2909,10 @@
     </row>
     <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E88" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F88" s="32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G88" s="38" t="s">
         <v>37</v>
@@ -2956,7 +2921,7 @@
         <v>38</v>
       </c>
       <c r="I88" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3010,44 +2975,44 @@
     </row>
     <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D96" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="E96" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="D96" s="40" t="s">
+      <c r="F96" s="41" t="s">
         <v>123</v>
-      </c>
-      <c r="E96" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="F96" s="41" t="s">
-        <v>125</v>
       </c>
       <c r="G96" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H96" s="42" t="s">
+      <c r="H96" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="I96" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="I96" s="13" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="97" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D97" s="43"/>
-      <c r="E97" s="43"/>
+      <c r="D97" s="42"/>
+      <c r="E97" s="42"/>
       <c r="F97" s="41"/>
-      <c r="G97" s="44" t="n">
+      <c r="G97" s="43" t="n">
         <v>26</v>
       </c>
-      <c r="H97" s="45" t="s">
+      <c r="H97" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I97" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="I97" s="29" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D98" s="43"/>
-      <c r="E98" s="43"/>
+      <c r="D98" s="42"/>
+      <c r="E98" s="42"/>
       <c r="F98" s="41"/>
       <c r="G98" s="35"/>
       <c r="H98" s="10" t="s">
@@ -3055,8 +3020,8 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D99" s="43"/>
-      <c r="E99" s="43"/>
+      <c r="D99" s="42"/>
+      <c r="E99" s="42"/>
       <c r="F99" s="41"/>
       <c r="G99" s="35"/>
       <c r="H99" s="10" t="s">
@@ -3064,8 +3029,8 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D100" s="43"/>
-      <c r="E100" s="43"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
       <c r="F100" s="41"/>
       <c r="G100" s="35"/>
       <c r="H100" s="10" t="s">
@@ -3073,128 +3038,128 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D101" s="43"/>
-      <c r="E101" s="43" t="s">
+      <c r="D101" s="42"/>
+      <c r="E101" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="F101" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="G101" s="44" t="n">
+        <v>23</v>
+      </c>
+      <c r="H101" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="F101" s="41" t="s">
+      <c r="I101" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="G101" s="46" t="n">
-        <v>23</v>
-      </c>
-      <c r="H101" s="39" t="s">
+    </row>
+    <row r="102" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D102" s="42"/>
+      <c r="E102" s="42"/>
+      <c r="F102" s="41"/>
+      <c r="G102" s="46" t="n">
+        <v>26</v>
+      </c>
+      <c r="H102" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I102" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D103" s="42"/>
+      <c r="E103" s="42"/>
+      <c r="F103" s="41"/>
+      <c r="G103" s="47" t="n">
+        <v>49</v>
+      </c>
+      <c r="H103" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="I101" s="47" t="s">
+      <c r="I103" s="13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D102" s="43"/>
-      <c r="E102" s="43"/>
-      <c r="F102" s="41"/>
-      <c r="G102" s="48" t="n">
-        <v>26</v>
-      </c>
-      <c r="H102" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="I102" s="29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D103" s="43"/>
-      <c r="E103" s="43"/>
-      <c r="F103" s="41"/>
-      <c r="G103" s="49" t="n">
-        <v>49</v>
-      </c>
-      <c r="H103" s="45" t="s">
+    <row r="104" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D104" s="42"/>
+      <c r="E104" s="42"/>
+      <c r="F104" s="41"/>
+      <c r="G104" s="47" t="n">
+        <v>50</v>
+      </c>
+      <c r="H104" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="I103" s="13" t="s">
+      <c r="I104" s="13" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D104" s="43"/>
-      <c r="E104" s="43"/>
-      <c r="F104" s="41"/>
-      <c r="G104" s="49" t="n">
-        <v>50</v>
-      </c>
-      <c r="H104" s="45" t="s">
+    <row r="105" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D105" s="42"/>
+      <c r="E105" s="42"/>
+      <c r="F105" s="41"/>
+      <c r="G105" s="47" t="n">
+        <v>51</v>
+      </c>
+      <c r="H105" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="I104" s="13" t="s">
+      <c r="I105" s="13" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D105" s="43"/>
-      <c r="E105" s="43"/>
-      <c r="F105" s="41"/>
-      <c r="G105" s="49" t="n">
-        <v>51</v>
-      </c>
-      <c r="H105" s="45" t="s">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D106" s="42"/>
+      <c r="E106" s="42"/>
+      <c r="F106" s="41"/>
+      <c r="G106" s="49" t="n">
+        <v>33</v>
+      </c>
+      <c r="H106" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="I105" s="13" t="s">
+      <c r="I106" s="0" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D106" s="43"/>
-      <c r="E106" s="43"/>
-      <c r="F106" s="41"/>
-      <c r="G106" s="50" t="n">
-        <v>33</v>
-      </c>
-      <c r="H106" s="33" t="s">
+    <row r="107" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D107" s="42"/>
+      <c r="E107" s="42"/>
+      <c r="F107" s="41"/>
+      <c r="G107" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="H107" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="I107" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D108" s="42"/>
+      <c r="E108" s="42"/>
+      <c r="F108" s="41"/>
+      <c r="G108" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="H108" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="I108" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D109" s="42"/>
+      <c r="E109" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="I106" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D107" s="43"/>
-      <c r="E107" s="43"/>
-      <c r="F107" s="41"/>
-      <c r="G107" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="H107" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="I107" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D108" s="43"/>
-      <c r="E108" s="43"/>
-      <c r="F108" s="41"/>
-      <c r="G108" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="H108" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="I108" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D109" s="43"/>
-      <c r="E109" s="43" t="s">
-        <v>138</v>
-      </c>
       <c r="F109" s="41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G109" s="38" t="s">
         <v>37</v>
@@ -3203,26 +3168,26 @@
         <v>38</v>
       </c>
       <c r="I109" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D110" s="43"/>
-      <c r="E110" s="43"/>
+      <c r="D110" s="42"/>
+      <c r="E110" s="42"/>
       <c r="F110" s="41"/>
       <c r="G110" s="34" t="n">
         <v>23</v>
       </c>
       <c r="H110" s="34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I110" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D111" s="43"/>
-      <c r="E111" s="43"/>
+      <c r="D111" s="42"/>
+      <c r="E111" s="42"/>
       <c r="F111" s="41"/>
       <c r="G111" s="35"/>
       <c r="H111" s="10" t="s">
@@ -3230,8 +3195,8 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D112" s="43"/>
-      <c r="E112" s="43"/>
+      <c r="D112" s="42"/>
+      <c r="E112" s="42"/>
       <c r="F112" s="41"/>
       <c r="G112" s="35"/>
       <c r="H112" s="10" t="s">
@@ -3239,8 +3204,8 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D113" s="43"/>
-      <c r="E113" s="43"/>
+      <c r="D113" s="42"/>
+      <c r="E113" s="42"/>
       <c r="F113" s="41"/>
       <c r="G113" s="35"/>
       <c r="H113" s="10" t="s">
@@ -3248,8 +3213,8 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D114" s="43"/>
-      <c r="E114" s="43"/>
+      <c r="D114" s="42"/>
+      <c r="E114" s="42"/>
       <c r="F114" s="41"/>
       <c r="G114" s="35"/>
       <c r="H114" s="10" t="s">
@@ -3257,8 +3222,8 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D115" s="43"/>
-      <c r="E115" s="43"/>
+      <c r="D115" s="42"/>
+      <c r="E115" s="42"/>
       <c r="F115" s="41"/>
       <c r="G115" s="35"/>
       <c r="H115" s="10" t="s">
@@ -3266,8 +3231,8 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D116" s="43"/>
-      <c r="E116" s="43"/>
+      <c r="D116" s="42"/>
+      <c r="E116" s="42"/>
       <c r="F116" s="41"/>
       <c r="G116" s="35"/>
       <c r="H116" s="10" t="s">
@@ -3276,31 +3241,31 @@
     </row>
     <row r="117" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C117" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="D117" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E117" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="F117" s="32" t="s">
         <v>141</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F117" s="32" t="s">
-        <v>143</v>
       </c>
       <c r="G117" s="23" t="n">
         <v>44</v>
       </c>
       <c r="H117" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="I117" s="51" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+      <c r="I117" s="50" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3309,10 +3274,10 @@
         <v>45</v>
       </c>
       <c r="H118" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="I118" s="52" t="s">
-        <v>147</v>
+        <v>144</v>
+      </c>
+      <c r="I118" s="51" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3321,10 +3286,10 @@
         <v>46</v>
       </c>
       <c r="H119" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="I119" s="53" t="s">
-        <v>149</v>
+        <v>146</v>
+      </c>
+      <c r="I119" s="52" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3332,11 +3297,11 @@
       <c r="G120" s="35" t="n">
         <v>47</v>
       </c>
-      <c r="H120" s="54" t="s">
-        <v>150</v>
+      <c r="H120" s="53" t="s">
+        <v>148</v>
       </c>
       <c r="I120" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3344,11 +3309,11 @@
       <c r="G121" s="35" t="n">
         <v>49</v>
       </c>
-      <c r="H121" s="54" t="s">
-        <v>130</v>
+      <c r="H121" s="53" t="s">
+        <v>128</v>
       </c>
       <c r="I121" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3370,23 +3335,23 @@
       <c r="H124" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I124" s="53"/>
+      <c r="I124" s="52"/>
     </row>
     <row r="125" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E125" s="0" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G125" s="23" t="n">
         <v>50</v>
       </c>
       <c r="H125" s="4" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="I125" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3397,7 +3362,7 @@
       <c r="H126" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I126" s="54" t="s">
+      <c r="I126" s="53" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3406,11 +3371,11 @@
       <c r="G127" s="35" t="n">
         <v>37</v>
       </c>
-      <c r="H127" s="55" t="s">
+      <c r="H127" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="I127" s="52" t="s">
         <v>154</v>
-      </c>
-      <c r="I127" s="53" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3418,11 +3383,11 @@
       <c r="G128" s="35" t="n">
         <v>40</v>
       </c>
-      <c r="H128" s="54" t="s">
+      <c r="H128" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="I128" s="52" t="s">
         <v>156</v>
-      </c>
-      <c r="I128" s="53" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3430,23 +3395,23 @@
       <c r="G129" s="35" t="n">
         <v>42</v>
       </c>
-      <c r="H129" s="54" t="s">
+      <c r="H129" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="I129" s="52" t="s">
         <v>158</v>
-      </c>
-      <c r="I129" s="53" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F130" s="5"/>
-      <c r="G130" s="49" t="n">
+      <c r="G130" s="47" t="n">
         <v>50</v>
       </c>
-      <c r="H130" s="45" t="s">
-        <v>132</v>
+      <c r="H130" s="48" t="s">
+        <v>130</v>
       </c>
       <c r="I130" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3458,148 +3423,148 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F132" s="5"/>
-      <c r="G132" s="56"/>
+      <c r="G132" s="55"/>
       <c r="H132" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C133" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D133" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="D133" s="57" t="s">
+      <c r="E133" s="56" t="s">
         <v>161</v>
       </c>
-      <c r="E133" s="57" t="s">
+      <c r="F133" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="F133" s="58" t="s">
+      <c r="G133" s="58"/>
+      <c r="H133" s="59"/>
+      <c r="I133" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="G133" s="59"/>
-      <c r="H133" s="60"/>
-      <c r="I133" s="61" t="s">
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D134" s="61"/>
+      <c r="E134" s="61"/>
+      <c r="F134" s="57"/>
+      <c r="G134" s="62"/>
+      <c r="H134" s="63"/>
+      <c r="I134" s="60"/>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D135" s="61" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D134" s="62"/>
-      <c r="E134" s="62"/>
-      <c r="F134" s="58"/>
-      <c r="G134" s="63"/>
-      <c r="H134" s="64"/>
-      <c r="I134" s="61"/>
-    </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D135" s="62" t="s">
-        <v>165</v>
-      </c>
-      <c r="E135" s="62"/>
-      <c r="F135" s="58"/>
-      <c r="G135" s="63"/>
-      <c r="H135" s="64"/>
-      <c r="I135" s="61"/>
+      <c r="E135" s="61"/>
+      <c r="F135" s="57"/>
+      <c r="G135" s="62"/>
+      <c r="H135" s="63"/>
+      <c r="I135" s="60"/>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D136" s="64"/>
-      <c r="E136" s="64"/>
-      <c r="F136" s="58"/>
-      <c r="G136" s="63"/>
-      <c r="H136" s="64"/>
-      <c r="I136" s="61"/>
+      <c r="D136" s="63"/>
+      <c r="E136" s="63"/>
+      <c r="F136" s="57"/>
+      <c r="G136" s="62"/>
+      <c r="H136" s="63"/>
+      <c r="I136" s="60"/>
     </row>
     <row r="137" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D137" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D137" s="4" t="s">
+      <c r="E137" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E137" s="4" t="s">
+      <c r="F137" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="F137" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="G137" s="23" t="n">
         <v>37</v>
       </c>
-      <c r="H137" s="65" t="s">
+      <c r="H137" s="64" t="s">
+        <v>153</v>
+      </c>
+      <c r="I137" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="I137" s="53" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="138" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D138" s="66"/>
-      <c r="E138" s="66"/>
+      <c r="D138" s="65"/>
+      <c r="E138" s="65"/>
       <c r="F138" s="5"/>
       <c r="G138" s="35" t="n">
         <v>39</v>
       </c>
-      <c r="H138" s="54" t="s">
+      <c r="H138" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="I138" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="I138" s="13" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="139" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D139" s="67"/>
-      <c r="E139" s="67"/>
+      <c r="D139" s="66"/>
+      <c r="E139" s="66"/>
       <c r="F139" s="5"/>
       <c r="G139" s="35" t="n">
         <v>40</v>
       </c>
-      <c r="H139" s="54" t="s">
+      <c r="H139" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="I139" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="I139" s="53" t="s">
-        <v>157</v>
-      </c>
     </row>
     <row r="140" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D140" s="66"/>
-      <c r="E140" s="66"/>
+      <c r="D140" s="65"/>
+      <c r="E140" s="65"/>
       <c r="F140" s="5"/>
       <c r="G140" s="35" t="n">
         <v>42</v>
       </c>
-      <c r="H140" s="54" t="s">
+      <c r="H140" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="I140" s="52" t="s">
         <v>158</v>
-      </c>
-      <c r="I140" s="53" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B141" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="C141" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C141" s="4" t="s">
+      <c r="D141" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D141" s="4" t="s">
+      <c r="E141" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E141" s="4" t="s">
+      <c r="F141" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="F141" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="G141" s="23" t="n">
         <v>50</v>
       </c>
       <c r="H141" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I141" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3607,11 +3572,11 @@
       <c r="G142" s="35" t="n">
         <v>37</v>
       </c>
-      <c r="H142" s="55" t="s">
+      <c r="H142" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="I142" s="52" t="s">
         <v>154</v>
-      </c>
-      <c r="I142" s="53" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3619,11 +3584,11 @@
       <c r="G143" s="35" t="n">
         <v>40</v>
       </c>
-      <c r="H143" s="54" t="s">
+      <c r="H143" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="I143" s="52" t="s">
         <v>156</v>
-      </c>
-      <c r="I143" s="53" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3668,7 +3633,7 @@
         <v>13</v>
       </c>
       <c r="H147" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I147" s="13" t="s">
         <v>68</v>
@@ -3683,29 +3648,29 @@
     </row>
     <row r="149" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C149" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D149" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D149" s="4" t="s">
+      <c r="E149" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E149" s="4" t="s">
+      <c r="F149" s="67" t="s">
         <v>181</v>
       </c>
-      <c r="F149" s="68" t="s">
-        <v>182</v>
-      </c>
-      <c r="G149" s="69" t="n">
+      <c r="G149" s="68" t="n">
         <v>17</v>
       </c>
       <c r="H149" s="4" t="s">
-        <v>183</v>
+        <v>44</v>
       </c>
       <c r="I149" s="13" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F150" s="68"/>
+      <c r="F150" s="67"/>
       <c r="G150" s="6" t="n">
         <v>18</v>
       </c>
@@ -3717,19 +3682,19 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F151" s="68"/>
+      <c r="F151" s="67"/>
       <c r="G151" s="6" t="n">
         <v>13</v>
       </c>
       <c r="H151" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I151" s="13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F152" s="68"/>
+      <c r="F152" s="67"/>
       <c r="G152" s="6" t="n">
         <v>14</v>
       </c>
@@ -3741,7 +3706,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F153" s="68"/>
+      <c r="F153" s="67"/>
       <c r="G153" s="6" t="n">
         <v>15</v>
       </c>
@@ -3753,21 +3718,21 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F154" s="68"/>
+      <c r="F154" s="67"/>
       <c r="G154" s="6"/>
       <c r="H154" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F155" s="68"/>
+      <c r="F155" s="67"/>
       <c r="G155" s="6"/>
       <c r="H155" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F156" s="68"/>
+      <c r="F156" s="67"/>
       <c r="G156" s="6"/>
       <c r="H156" s="10" t="s">
         <v>23</v>
@@ -3775,19 +3740,19 @@
     </row>
     <row r="157" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E157" s="0" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F157" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G157" s="23" t="n">
         <v>50</v>
       </c>
       <c r="H157" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I157" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3795,11 +3760,11 @@
       <c r="G158" s="35" t="n">
         <v>37</v>
       </c>
-      <c r="H158" s="55" t="s">
+      <c r="H158" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="I158" s="52" t="s">
         <v>154</v>
-      </c>
-      <c r="I158" s="53" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3807,11 +3772,11 @@
       <c r="G159" s="35" t="n">
         <v>40</v>
       </c>
-      <c r="H159" s="54" t="s">
+      <c r="H159" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="I159" s="52" t="s">
         <v>156</v>
-      </c>
-      <c r="I159" s="53" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3820,9 +3785,9 @@
         <v>21</v>
       </c>
       <c r="H160" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I160" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="I160" s="53" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3856,65 +3821,65 @@
     </row>
     <row r="165" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E165" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="F165" s="70" t="s">
-        <v>187</v>
+        <v>184</v>
+      </c>
+      <c r="F165" s="69" t="s">
+        <v>185</v>
       </c>
       <c r="G165" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H165" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I165" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F166" s="70"/>
+      <c r="F166" s="69"/>
       <c r="G166" s="35"/>
       <c r="H166" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F167" s="70"/>
+      <c r="F167" s="69"/>
       <c r="G167" s="35"/>
       <c r="H167" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F168" s="70"/>
+      <c r="F168" s="69"/>
       <c r="G168" s="35"/>
       <c r="H168" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F169" s="70"/>
+      <c r="F169" s="69"/>
       <c r="G169" s="35"/>
       <c r="H169" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F170" s="70"/>
+      <c r="F170" s="69"/>
       <c r="G170" s="35"/>
       <c r="H170" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F171" s="70"/>
+      <c r="F171" s="69"/>
       <c r="G171" s="35"/>
       <c r="H171" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F172" s="70"/>
+      <c r="F172" s="69"/>
       <c r="G172" s="35"/>
       <c r="H172" s="10" t="s">
         <v>23</v>

</xml_diff>